<commit_message>
Verschieben einiger Dokumente in andere Ordner
</commit_message>
<xml_diff>
--- a/Documents/Stundenlisten/Stunden.xlsx
+++ b/Documents/Stundenlisten/Stunden.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12443"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Datum</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>technische Dokumentation</t>
+  </si>
+  <si>
+    <t>Erstellen der Kommunikationsbibliothek und der Server Applikation</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
@@ -326,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -377,6 +386,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -657,557 +687,685 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="102.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="7.53125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="13">
         <v>42630</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="25">
+        <v>7</v>
+      </c>
+      <c r="D2" s="29">
         <v>1.5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>42711</v>
       </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="26">
+        <v>7</v>
+      </c>
+      <c r="D3" s="30">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3">
         <v>42748</v>
       </c>
-      <c r="C4" s="4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="26">
+        <v>8</v>
+      </c>
+      <c r="D4" s="30">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3">
-        <v>42764</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42760</v>
+      </c>
+      <c r="C5" s="26">
+        <v>2</v>
+      </c>
+      <c r="D5" s="30">
+        <v>3.5</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3">
-        <v>42777</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42764</v>
+      </c>
+      <c r="C6" s="26">
+        <v>3</v>
+      </c>
+      <c r="D6" s="30">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
+        <v>42777</v>
+      </c>
+      <c r="C7" s="26">
+        <v>2</v>
+      </c>
+      <c r="D7" s="30">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
         <v>42778</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="26">
+        <v>2</v>
+      </c>
+      <c r="D8" s="30">
         <v>1</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9" s="26"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="6"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="26"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" s="26"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="6"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" s="26"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="13">
-        <v>42630</v>
-      </c>
-      <c r="C15" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="26"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="6"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="3">
-        <v>42711</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="13">
+        <v>42630</v>
+      </c>
+      <c r="C16" s="25">
+        <v>7</v>
+      </c>
+      <c r="D16" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="3">
-        <v>42764</v>
-      </c>
-      <c r="C17" s="4">
-        <v>2</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>42711</v>
+      </c>
+      <c r="C17" s="26">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="22">
-        <v>42768</v>
-      </c>
-      <c r="C18" s="2">
-        <v>2</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="3">
+        <v>42764</v>
+      </c>
+      <c r="C18" s="26">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="22">
+        <v>42768</v>
+      </c>
+      <c r="C19" s="28">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3">
         <v>42779</v>
       </c>
-      <c r="C19" s="4">
-        <v>3</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="C20" s="26">
+        <v>3</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="26"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="6"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="26"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C23" s="26"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="6"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C24" s="26"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C25" s="26"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="6"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C26" s="26"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C27" s="26"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="6"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="21" t="s">
+      <c r="C28" s="26"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B31" s="13">
         <v>42711</v>
       </c>
-      <c r="C30" s="14">
-        <v>2</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="C31" s="25">
+        <v>7</v>
+      </c>
+      <c r="D31" s="14">
+        <v>2</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="3">
-        <v>42762</v>
-      </c>
-      <c r="C31" s="20">
-        <v>1.5</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="3">
-        <v>42774</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42762</v>
+      </c>
+      <c r="C32" s="26">
+        <v>2</v>
+      </c>
+      <c r="D32" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="3">
-        <v>42778</v>
-      </c>
-      <c r="C33" s="4">
-        <v>2</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42774</v>
+      </c>
+      <c r="C33" s="26">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="3">
+        <v>42778</v>
+      </c>
+      <c r="C34" s="26">
+        <v>3</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="3">
         <v>42779</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C35" s="26">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4">
         <v>1.5</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="6"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C36" s="26"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C37" s="26"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="6"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C38" s="26"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C39" s="26"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="6"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C40" s="26"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C41" s="26"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="6"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C42" s="26"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="12" t="s">
+      <c r="C43" s="26"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" s="6"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="13">
+      <c r="B46" s="13">
         <v>42630</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C46" s="25">
+        <v>7</v>
+      </c>
+      <c r="D46" s="14">
         <v>1.5</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="E46" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="3">
-        <v>43076</v>
-      </c>
-      <c r="C46" s="4">
-        <v>2</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B47" s="3">
-        <v>42748</v>
-      </c>
-      <c r="C47" s="4">
-        <v>1</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43076</v>
+      </c>
+      <c r="C47" s="26">
+        <v>7</v>
+      </c>
+      <c r="D47" s="4">
+        <v>2</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="3">
-        <v>42764</v>
-      </c>
-      <c r="C48" s="4">
-        <v>2</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42748</v>
+      </c>
+      <c r="C48" s="26">
+        <v>3</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="3">
-        <v>42778</v>
-      </c>
-      <c r="C49" s="4">
-        <v>3</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42760</v>
+      </c>
+      <c r="C49" s="26">
+        <v>3</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="3">
+        <v>42778</v>
+      </c>
+      <c r="C50" s="26">
+        <v>3</v>
+      </c>
+      <c r="D50" s="4">
+        <v>3</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="3">
         <v>42779</v>
       </c>
-      <c r="C50" s="4">
-        <v>2</v>
-      </c>
-      <c r="D50" s="7" t="s">
+      <c r="C51" s="26">
+        <v>3</v>
+      </c>
+      <c r="D51" s="4">
+        <v>2</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="6"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="6"/>
       <c r="B52" s="5"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C52" s="26"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="7"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="6"/>
       <c r="B53" s="5"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="6"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="7"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="B54" s="5"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="7"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C54" s="26"/>
+      <c r="D54" s="30">
+        <f>SUM(D2:D51)</f>
+        <v>46</v>
+      </c>
+      <c r="E54" s="7"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="6"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C55" s="26"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="6"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="7"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C56" s="26"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="6"/>
       <c r="B57" s="5"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="7"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C57" s="26"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="6"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="8"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="11"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="7"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" s="6"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>